<commit_message>
Atualização Planilha View Hard-Code
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/View_Report_MIS.xlsx
+++ b/Documentação/Planilhas/View_Report_MIS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="2895" tabRatio="311" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="2895" tabRatio="270" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="View" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4473" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4566" uniqueCount="1068">
   <si>
     <t>TABLE_CATALOG</t>
   </si>
@@ -3443,7 +3443,34 @@
     <t>Consome Direto do SIGE</t>
   </si>
   <si>
-    <t>Validar Mudança Garantia Extendida</t>
+    <t>Devido a regra para carga de SKU, o cenário atual não muda apenas que o mesmo SKU para GE são os mesmo para todos os SKU's</t>
+  </si>
+  <si>
+    <t>Conforme visualização de uso, deverá ser desativado na migração do LN</t>
+  </si>
+  <si>
+    <t>Deverá ser modificada, atentando-se para teste na qt_estoque e valor CMV, pois dada a mudança na view e inclusão de novo campo na Fato Estoque Sige, não foi possivel fazer teste com massa de dados em Desenv</t>
+  </si>
+  <si>
+    <t>Substituir Relatorio</t>
+  </si>
+  <si>
+    <t>Substituir procedure mapeada scrip mudança MIS_RELATORIO</t>
+  </si>
+  <si>
+    <t>Alerta!</t>
+  </si>
+  <si>
+    <t>Verificar no front mudança de regra de procedure que executa o relatório</t>
+  </si>
+  <si>
+    <t>Substituir DataSet Filial, modificando pelo numero da companhia vigente no LN, em DEV é 201</t>
+  </si>
+  <si>
+    <t>Conforme orientação do Patrick, manter relatório em Hold até definição de fonte para extração (LN ou BI)</t>
+  </si>
+  <si>
+    <t>Substituir Dataset DSetRelatorio, devido a mudança da query, no qual sofreu alteração no STATUS do Item</t>
   </si>
 </sst>
 </file>
@@ -3623,7 +3650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3744,7 +3771,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15533,8 +15569,8 @@
   <dimension ref="A1:J197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15547,6 +15583,8 @@
     <col min="6" max="6" width="44" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" style="12" customWidth="1"/>
     <col min="8" max="8" width="71.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
@@ -17211,7 +17249,7 @@
       </c>
       <c r="I64" s="35"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:10">
       <c r="A65" s="24" t="s">
         <v>720</v>
       </c>
@@ -17238,7 +17276,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="60">
+    <row r="66" spans="1:10" ht="60">
       <c r="A66" s="24" t="s">
         <v>720</v>
       </c>
@@ -17265,7 +17303,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:10">
       <c r="A67" s="22" t="s">
         <v>720</v>
       </c>
@@ -17292,7 +17330,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:10">
       <c r="A68" s="22" t="s">
         <v>730</v>
       </c>
@@ -17317,7 +17355,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:10">
       <c r="A69" s="24" t="s">
         <v>735</v>
       </c>
@@ -17346,7 +17384,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:10">
       <c r="A70" s="9" t="s">
         <v>735</v>
       </c>
@@ -17375,7 +17413,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:10">
       <c r="A71" s="9" t="s">
         <v>735</v>
       </c>
@@ -17404,7 +17442,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:10">
       <c r="A72" s="9" t="s">
         <v>735</v>
       </c>
@@ -17433,7 +17471,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:10">
       <c r="A73" s="9" t="s">
         <v>735</v>
       </c>
@@ -17462,7 +17500,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:10">
       <c r="A74" s="24" t="s">
         <v>762</v>
       </c>
@@ -17489,7 +17527,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:10">
       <c r="A75" s="24" t="s">
         <v>769</v>
       </c>
@@ -17516,7 +17554,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="135">
+    <row r="76" spans="1:10" ht="135">
       <c r="A76" s="24" t="s">
         <v>769</v>
       </c>
@@ -17543,7 +17581,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:10">
       <c r="A77" s="24" t="s">
         <v>769</v>
       </c>
@@ -17570,7 +17608,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:10">
       <c r="A78" s="24" t="s">
         <v>769</v>
       </c>
@@ -17597,8 +17635,8 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="24" t="s">
+    <row r="79" spans="1:10">
+      <c r="A79" s="42" t="s">
         <v>776</v>
       </c>
       <c r="B79" s="14" t="s">
@@ -17623,9 +17661,12 @@
       <c r="I79" s="35" t="s">
         <v>1057</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="24" t="s">
+      <c r="J79" s="41" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="42" t="s">
         <v>776</v>
       </c>
       <c r="B80" s="14" t="s">
@@ -17650,9 +17691,10 @@
       <c r="I80" s="35" t="s">
         <v>1057</v>
       </c>
+      <c r="J80" s="41"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="24" t="s">
+      <c r="A81" s="42" t="s">
         <v>776</v>
       </c>
       <c r="B81" s="14" t="s">
@@ -17677,6 +17719,7 @@
       <c r="I81" s="35" t="s">
         <v>1057</v>
       </c>
+      <c r="J81" s="41"/>
     </row>
     <row r="82" spans="1:10" ht="270">
       <c r="A82" s="29" t="s">
@@ -17918,7 +17961,9 @@
       <c r="H91" s="31" t="s">
         <v>820</v>
       </c>
-      <c r="I91" s="35"/>
+      <c r="I91" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="92" spans="1:10" ht="150">
       <c r="A92" s="30" t="s">
@@ -17939,7 +17984,9 @@
       <c r="H92" s="31" t="s">
         <v>819</v>
       </c>
-      <c r="I92" s="35"/>
+      <c r="I92" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="24" t="s">
@@ -17963,7 +18010,10 @@
         <v>828</v>
       </c>
       <c r="I93" s="35" t="s">
-        <v>1022</v>
+        <v>1061</v>
+      </c>
+      <c r="J93" s="41" t="s">
+        <v>1060</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -17987,7 +18037,10 @@
       <c r="H94" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="I94" s="35"/>
+      <c r="I94" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J94" s="41"/>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="24" t="s">
@@ -18011,8 +18064,9 @@
         <v>824</v>
       </c>
       <c r="I95" s="35" t="s">
-        <v>1022</v>
-      </c>
+        <v>1061</v>
+      </c>
+      <c r="J95" s="41"/>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="24" t="s">
@@ -18035,9 +18089,12 @@
       <c r="H96" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I96" s="35"/>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="I96" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J96" s="41"/>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="24" t="s">
         <v>825</v>
       </c>
@@ -18058,9 +18115,14 @@
       <c r="H97" s="21" t="s">
         <v>828</v>
       </c>
-      <c r="I97" s="35"/>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="I97" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J97" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="24" t="s">
         <v>825</v>
       </c>
@@ -18081,9 +18143,12 @@
       <c r="H98" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="I98" s="35"/>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="I98" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J98" s="41"/>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="24" t="s">
         <v>825</v>
       </c>
@@ -18105,10 +18170,11 @@
         <v>824</v>
       </c>
       <c r="I99" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+        <v>1061</v>
+      </c>
+      <c r="J99" s="41"/>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="24" t="s">
         <v>825</v>
       </c>
@@ -18129,9 +18195,12 @@
       <c r="H100" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I100" s="35"/>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="I100" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J100" s="41"/>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="24" t="s">
         <v>832</v>
       </c>
@@ -18154,9 +18223,14 @@
       <c r="H101" s="21" t="s">
         <v>828</v>
       </c>
-      <c r="I101" s="35"/>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="I101" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J101" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="24" t="s">
         <v>832</v>
       </c>
@@ -18179,9 +18253,12 @@
       <c r="H102" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="I102" s="35"/>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="I102" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J102" s="41"/>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="24" t="s">
         <v>832</v>
       </c>
@@ -18205,10 +18282,11 @@
         <v>824</v>
       </c>
       <c r="I103" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+        <v>1062</v>
+      </c>
+      <c r="J103" s="41"/>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="24" t="s">
         <v>832</v>
       </c>
@@ -18231,9 +18309,12 @@
       <c r="H104" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I104" s="35"/>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="I104" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J104" s="41"/>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="24" t="s">
         <v>834</v>
       </c>
@@ -18256,9 +18337,14 @@
       <c r="H105" s="21" t="s">
         <v>828</v>
       </c>
-      <c r="I105" s="35"/>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="I105" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J105" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="24" t="s">
         <v>834</v>
       </c>
@@ -18282,10 +18368,11 @@
         <v>824</v>
       </c>
       <c r="I106" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+        <v>1062</v>
+      </c>
+      <c r="J106" s="41"/>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="24" t="s">
         <v>834</v>
       </c>
@@ -18308,9 +18395,12 @@
       <c r="H107" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I107" s="35"/>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="I107" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J107" s="41"/>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="24" t="s">
         <v>834</v>
       </c>
@@ -18333,9 +18423,12 @@
       <c r="H108" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="I108" s="35"/>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="I108" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J108" s="41"/>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="9" t="s">
         <v>837</v>
       </c>
@@ -18358,9 +18451,14 @@
       <c r="H109" s="21" t="s">
         <v>828</v>
       </c>
-      <c r="I109" s="35"/>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="I109" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J109" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="9" t="s">
         <v>837</v>
       </c>
@@ -18384,10 +18482,11 @@
         <v>824</v>
       </c>
       <c r="I110" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+        <v>1062</v>
+      </c>
+      <c r="J110" s="41"/>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="9" t="s">
         <v>837</v>
       </c>
@@ -18410,9 +18509,12 @@
       <c r="H111" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I111" s="35"/>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="I111" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J111" s="41"/>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="9" t="s">
         <v>837</v>
       </c>
@@ -18435,9 +18537,12 @@
       <c r="H112" s="21" t="s">
         <v>823</v>
       </c>
-      <c r="I112" s="35"/>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="I112" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J112" s="41"/>
+    </row>
+    <row r="113" spans="1:10" ht="15" customHeight="1">
       <c r="A113" s="24" t="s">
         <v>840</v>
       </c>
@@ -18458,9 +18563,14 @@
       <c r="H113" s="21" t="s">
         <v>843</v>
       </c>
-      <c r="I113" s="35"/>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="I113" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J113" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="24" t="s">
         <v>840</v>
       </c>
@@ -18481,9 +18591,12 @@
       <c r="H114" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I114" s="35"/>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="I114" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J114" s="41"/>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="24" t="s">
         <v>840</v>
       </c>
@@ -18505,10 +18618,11 @@
         <v>824</v>
       </c>
       <c r="I115" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+        <v>1061</v>
+      </c>
+      <c r="J115" s="41"/>
+    </row>
+    <row r="116" spans="1:10" ht="15" customHeight="1">
       <c r="A116" s="9" t="s">
         <v>846</v>
       </c>
@@ -18531,9 +18645,14 @@
       <c r="H116" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I116" s="35"/>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="I116" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J116" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="9" t="s">
         <v>846</v>
       </c>
@@ -18557,10 +18676,11 @@
         <v>824</v>
       </c>
       <c r="I117" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+        <v>1062</v>
+      </c>
+      <c r="J117" s="41"/>
+    </row>
+    <row r="118" spans="1:10" ht="15" customHeight="1">
       <c r="A118" s="9" t="s">
         <v>848</v>
       </c>
@@ -18583,9 +18703,14 @@
       <c r="H118" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I118" s="35"/>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="I118" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J118" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="9" t="s">
         <v>848</v>
       </c>
@@ -18609,10 +18734,11 @@
         <v>824</v>
       </c>
       <c r="I119" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>1062</v>
+      </c>
+      <c r="J119" s="41"/>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="24" t="s">
         <v>848</v>
       </c>
@@ -18633,9 +18759,12 @@
       <c r="H120" s="21" t="s">
         <v>851</v>
       </c>
-      <c r="I120" s="35"/>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="I120" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J120" s="41"/>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="24" t="s">
         <v>853</v>
       </c>
@@ -18656,9 +18785,14 @@
       <c r="H121" s="21" t="s">
         <v>843</v>
       </c>
-      <c r="I121" s="35"/>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="I121" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J121" s="41" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="24" t="s">
         <v>853</v>
       </c>
@@ -18680,10 +18814,11 @@
         <v>824</v>
       </c>
       <c r="I122" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>1061</v>
+      </c>
+      <c r="J122" s="41"/>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="24" t="s">
         <v>853</v>
       </c>
@@ -18704,9 +18839,12 @@
       <c r="H123" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="I123" s="35"/>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="I123" s="35" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J123" s="41"/>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="9" t="s">
         <v>854</v>
       </c>
@@ -18727,9 +18865,11 @@
       <c r="H124" s="21" t="s">
         <v>856</v>
       </c>
-      <c r="I124" s="35"/>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="I124" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="9" t="s">
         <v>854</v>
       </c>
@@ -18750,9 +18890,11 @@
       <c r="H125" s="21" t="s">
         <v>857</v>
       </c>
-      <c r="I125" s="35"/>
-    </row>
-    <row r="126" spans="1:9" ht="45">
+      <c r="I125" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="45">
       <c r="A126" s="9" t="s">
         <v>854</v>
       </c>
@@ -18773,9 +18915,11 @@
       <c r="H126" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="I126" s="35"/>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="I126" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="9" t="s">
         <v>854</v>
       </c>
@@ -18796,9 +18940,11 @@
       <c r="H127" s="21" t="s">
         <v>858</v>
       </c>
-      <c r="I127" s="35"/>
-    </row>
-    <row r="128" spans="1:9" ht="45">
+      <c r="I127" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="45">
       <c r="A128" s="24" t="s">
         <v>854</v>
       </c>
@@ -18817,7 +18963,9 @@
       <c r="H128" s="21" t="s">
         <v>862</v>
       </c>
-      <c r="I128" s="35"/>
+      <c r="I128" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="129" spans="1:9" ht="45">
       <c r="A129" s="24" t="s">
@@ -18838,7 +18986,9 @@
       <c r="H129" s="21" t="s">
         <v>862</v>
       </c>
-      <c r="I129" s="35"/>
+      <c r="I129" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="130" spans="1:9" ht="45">
       <c r="A130" s="24" t="s">
@@ -18859,7 +19009,9 @@
       <c r="H130" s="21" t="s">
         <v>864</v>
       </c>
-      <c r="I130" s="35"/>
+      <c r="I130" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="131" spans="1:9" ht="45">
       <c r="A131" s="23" t="s">
@@ -18880,7 +19032,9 @@
       <c r="H131" s="13" t="s">
         <v>864</v>
       </c>
-      <c r="I131" s="35"/>
+      <c r="I131" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="132" spans="1:9" ht="75">
       <c r="A132" s="24" t="s">
@@ -18901,7 +19055,9 @@
       <c r="H132" s="21" t="s">
         <v>866</v>
       </c>
-      <c r="I132" s="35"/>
+      <c r="I132" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="133" spans="1:9" ht="75">
       <c r="A133" s="24" t="s">
@@ -18922,7 +19078,9 @@
       <c r="H133" s="21" t="s">
         <v>866</v>
       </c>
-      <c r="I133" s="35"/>
+      <c r="I133" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="24" t="s">
@@ -18945,7 +19103,9 @@
       <c r="H134" s="21" t="s">
         <v>867</v>
       </c>
-      <c r="I134" s="35"/>
+      <c r="I134" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="24" t="s">
@@ -18969,7 +19129,7 @@
         <v>870</v>
       </c>
       <c r="I135" s="35" t="s">
-        <v>1023</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="45">
@@ -18991,7 +19151,9 @@
       <c r="H136" s="21" t="s">
         <v>874</v>
       </c>
-      <c r="I136" s="35"/>
+      <c r="I136" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="137" spans="1:9" ht="45">
       <c r="A137" s="24" t="s">
@@ -19012,7 +19174,9 @@
       <c r="H137" s="21" t="s">
         <v>874</v>
       </c>
-      <c r="I137" s="35"/>
+      <c r="I137" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="24" t="s">
@@ -19035,7 +19199,9 @@
       <c r="H138" s="21" t="s">
         <v>876</v>
       </c>
-      <c r="I138" s="35"/>
+      <c r="I138" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="24" t="s">
@@ -19060,7 +19226,9 @@
       <c r="H139" s="21" t="s">
         <v>882</v>
       </c>
-      <c r="I139" s="35"/>
+      <c r="I139" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="24" t="s">
@@ -19083,7 +19251,9 @@
       <c r="H140" s="21" t="s">
         <v>884</v>
       </c>
-      <c r="I140" s="35"/>
+      <c r="I140" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="24" t="s">
@@ -19106,7 +19276,9 @@
       <c r="H141" s="21" t="s">
         <v>891</v>
       </c>
-      <c r="I141" s="35"/>
+      <c r="I141" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="24" t="s">
@@ -19129,7 +19301,9 @@
       <c r="H142" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="I142" s="35"/>
+      <c r="I142" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="24" t="s">
@@ -19152,7 +19326,9 @@
       <c r="H143" s="21" t="s">
         <v>891</v>
       </c>
-      <c r="I143" s="35"/>
+      <c r="I143" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="24" t="s">
@@ -19175,7 +19351,9 @@
       <c r="H144" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="I144" s="35"/>
+      <c r="I144" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="24" t="s">
@@ -19198,7 +19376,9 @@
       <c r="H145" s="21" t="s">
         <v>899</v>
       </c>
-      <c r="I145" s="35"/>
+      <c r="I145" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="146" spans="1:9" ht="30">
       <c r="A146" s="24" t="s">
@@ -19221,7 +19401,9 @@
       <c r="H146" s="21" t="s">
         <v>903</v>
       </c>
-      <c r="I146" s="35"/>
+      <c r="I146" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="147" spans="1:9" ht="105">
       <c r="A147" s="24" t="s">
@@ -19243,7 +19425,7 @@
         <v>907</v>
       </c>
       <c r="I147" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="105">
@@ -19266,7 +19448,7 @@
         <v>907</v>
       </c>
       <c r="I148" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -19290,7 +19472,9 @@
       <c r="H149" s="21" t="s">
         <v>912</v>
       </c>
-      <c r="I149" s="35"/>
+      <c r="I149" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="24" t="s">
@@ -19313,7 +19497,9 @@
       <c r="H150" s="21" t="s">
         <v>914</v>
       </c>
-      <c r="I150" s="35"/>
+      <c r="I150" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="151" spans="1:9" ht="30">
       <c r="A151" s="27" t="s">
@@ -19336,7 +19522,9 @@
       <c r="H151" s="21" t="s">
         <v>917</v>
       </c>
-      <c r="I151" s="35"/>
+      <c r="I151" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="152" spans="1:9" ht="30">
       <c r="A152" s="27" t="s">
@@ -19359,7 +19547,9 @@
       <c r="H152" s="13" t="s">
         <v>918</v>
       </c>
-      <c r="I152" s="35"/>
+      <c r="I152" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="153" spans="1:9" ht="60">
       <c r="A153" s="27" t="s">
@@ -19382,7 +19572,9 @@
       <c r="H153" s="21" t="s">
         <v>921</v>
       </c>
-      <c r="I153" s="35"/>
+      <c r="I153" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="154" spans="1:9" ht="60">
       <c r="A154" s="27" t="s">
@@ -19405,7 +19597,9 @@
       <c r="H154" s="21" t="s">
         <v>923</v>
       </c>
-      <c r="I154" s="35"/>
+      <c r="I154" s="35" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="155" spans="1:9">
       <c r="A155" s="22" t="s">
@@ -19429,7 +19623,7 @@
         <v>926</v>
       </c>
       <c r="I155" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -19454,7 +19648,7 @@
         <v>927</v>
       </c>
       <c r="I156" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -19479,7 +19673,7 @@
         <v>928</v>
       </c>
       <c r="I157" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="60">
@@ -19504,7 +19698,7 @@
         <v>932</v>
       </c>
       <c r="I158" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="68.25" customHeight="1">
@@ -19529,7 +19723,7 @@
         <v>933</v>
       </c>
       <c r="I159" s="35" t="s">
-        <v>1022</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -19553,9 +19747,11 @@
       <c r="H160" s="21" t="s">
         <v>912</v>
       </c>
-      <c r="I160" s="35"/>
-    </row>
-    <row r="161" spans="1:9" ht="45">
+      <c r="I160" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="45">
       <c r="A161" s="22" t="s">
         <v>924</v>
       </c>
@@ -19574,9 +19770,11 @@
       <c r="H161" s="21" t="s">
         <v>935</v>
       </c>
-      <c r="I161" s="35"/>
-    </row>
-    <row r="162" spans="1:9">
+      <c r="I161" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162" s="22" t="s">
         <v>924</v>
       </c>
@@ -19597,9 +19795,11 @@
       <c r="H162" s="21" t="s">
         <v>936</v>
       </c>
-      <c r="I162" s="35"/>
-    </row>
-    <row r="163" spans="1:9">
+      <c r="I162" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163" s="22" t="s">
         <v>924</v>
       </c>
@@ -19620,9 +19820,11 @@
       <c r="H163" s="21" t="s">
         <v>938</v>
       </c>
-      <c r="I163" s="35"/>
-    </row>
-    <row r="164" spans="1:9" ht="90">
+      <c r="I163" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="90">
       <c r="A164" s="9" t="s">
         <v>939</v>
       </c>
@@ -19643,9 +19845,11 @@
       <c r="H164" s="21" t="s">
         <v>941</v>
       </c>
-      <c r="I164" s="35"/>
-    </row>
-    <row r="165" spans="1:9" ht="90">
+      <c r="I164" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="90">
       <c r="A165" s="22" t="s">
         <v>939</v>
       </c>
@@ -19666,9 +19870,11 @@
       <c r="H165" s="21" t="s">
         <v>943</v>
       </c>
-      <c r="I165" s="35"/>
-    </row>
-    <row r="166" spans="1:9">
+      <c r="I165" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166" s="24" t="s">
         <v>946</v>
       </c>
@@ -19689,9 +19895,11 @@
       <c r="H166" s="21" t="s">
         <v>995</v>
       </c>
-      <c r="I166" s="35"/>
-    </row>
-    <row r="167" spans="1:9" ht="60">
+      <c r="I166" s="35" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="60">
       <c r="A167" s="24" t="s">
         <v>946</v>
       </c>
@@ -19712,9 +19920,11 @@
       <c r="H167" s="21" t="s">
         <v>997</v>
       </c>
-      <c r="I167" s="35"/>
-    </row>
-    <row r="168" spans="1:9" ht="60">
+      <c r="I167" s="35" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="60">
       <c r="A168" s="24" t="s">
         <v>946</v>
       </c>
@@ -19735,9 +19945,11 @@
       <c r="H168" s="13" t="s">
         <v>999</v>
       </c>
-      <c r="I168" s="35"/>
-    </row>
-    <row r="169" spans="1:9" ht="60">
+      <c r="I168" s="35" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="60">
       <c r="A169" s="23" t="s">
         <v>946</v>
       </c>
@@ -19758,9 +19970,11 @@
       <c r="H169" s="21" t="s">
         <v>1000</v>
       </c>
-      <c r="I169" s="35"/>
-    </row>
-    <row r="170" spans="1:9">
+      <c r="I169" s="35" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170" s="24" t="s">
         <v>946</v>
       </c>
@@ -19781,9 +19995,11 @@
       <c r="H170" s="21" t="s">
         <v>1004</v>
       </c>
-      <c r="I170" s="35"/>
-    </row>
-    <row r="171" spans="1:9">
+      <c r="I170" s="35" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171" s="24" t="s">
         <v>946</v>
       </c>
@@ -19804,9 +20020,14 @@
       <c r="H171" s="21" t="s">
         <v>1005</v>
       </c>
-      <c r="I171" s="35"/>
-    </row>
-    <row r="172" spans="1:9" ht="135">
+      <c r="I171" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J171" s="43" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="135">
       <c r="A172" s="24" t="s">
         <v>946</v>
       </c>
@@ -19827,9 +20048,12 @@
       <c r="H172" s="21" t="s">
         <v>1008</v>
       </c>
-      <c r="I172" s="35"/>
-    </row>
-    <row r="173" spans="1:9" ht="135">
+      <c r="I172" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J172" s="43"/>
+    </row>
+    <row r="173" spans="1:10" ht="135">
       <c r="A173" s="24" t="s">
         <v>946</v>
       </c>
@@ -19850,9 +20074,12 @@
       <c r="H173" s="21" t="s">
         <v>1009</v>
       </c>
-      <c r="I173" s="35"/>
-    </row>
-    <row r="174" spans="1:9" ht="135">
+      <c r="I173" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J173" s="43"/>
+    </row>
+    <row r="174" spans="1:10" ht="135">
       <c r="A174" s="24" t="s">
         <v>946</v>
       </c>
@@ -19873,9 +20100,12 @@
       <c r="H174" s="21" t="s">
         <v>1012</v>
       </c>
-      <c r="I174" s="35"/>
-    </row>
-    <row r="175" spans="1:9" ht="135">
+      <c r="I174" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J174" s="43"/>
+    </row>
+    <row r="175" spans="1:10" ht="135">
       <c r="A175" s="24" t="s">
         <v>946</v>
       </c>
@@ -19896,9 +20126,12 @@
       <c r="H175" s="21" t="s">
         <v>1015</v>
       </c>
-      <c r="I175" s="35"/>
-    </row>
-    <row r="176" spans="1:9" ht="135">
+      <c r="I175" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J175" s="43"/>
+    </row>
+    <row r="176" spans="1:10" ht="135">
       <c r="A176" s="24" t="s">
         <v>946</v>
       </c>
@@ -19919,9 +20152,12 @@
       <c r="H176" s="21" t="s">
         <v>1016</v>
       </c>
-      <c r="I176" s="35"/>
-    </row>
-    <row r="177" spans="1:9">
+      <c r="I176" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J176" s="43"/>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177" s="24" t="s">
         <v>946</v>
       </c>
@@ -19942,9 +20178,12 @@
       <c r="H177" s="21" t="s">
         <v>1018</v>
       </c>
-      <c r="I177" s="35"/>
-    </row>
-    <row r="178" spans="1:9">
+      <c r="I177" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J177" s="43"/>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178" s="24" t="s">
         <v>946</v>
       </c>
@@ -19965,9 +20204,12 @@
       <c r="H178" s="21" t="s">
         <v>1020</v>
       </c>
-      <c r="I178" s="35"/>
-    </row>
-    <row r="179" spans="1:9">
+      <c r="I178" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J178" s="43"/>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179" s="24" t="s">
         <v>946</v>
       </c>
@@ -19988,9 +20230,12 @@
       <c r="H179" s="21" t="s">
         <v>1020</v>
       </c>
-      <c r="I179" s="35"/>
-    </row>
-    <row r="180" spans="1:9">
+      <c r="I179" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J179" s="43"/>
+    </row>
+    <row r="180" spans="1:10">
       <c r="A180" s="24" t="s">
         <v>946</v>
       </c>
@@ -20011,9 +20256,12 @@
       <c r="H180" s="21" t="s">
         <v>1018</v>
       </c>
-      <c r="I180" s="35"/>
-    </row>
-    <row r="181" spans="1:9">
+      <c r="I180" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J180" s="43"/>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181" s="23" t="s">
         <v>946</v>
       </c>
@@ -20034,9 +20282,12 @@
       <c r="H181" s="21" t="s">
         <v>1020</v>
       </c>
-      <c r="I181" s="35"/>
-    </row>
-    <row r="182" spans="1:9">
+      <c r="I181" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J181" s="43"/>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182" s="23" t="s">
         <v>946</v>
       </c>
@@ -20057,9 +20308,12 @@
       <c r="H182" s="21" t="s">
         <v>1020</v>
       </c>
-      <c r="I182" s="35"/>
-    </row>
-    <row r="183" spans="1:9" ht="30">
+      <c r="I182" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J182" s="43"/>
+    </row>
+    <row r="183" spans="1:10" ht="30">
       <c r="A183" s="23" t="s">
         <v>946</v>
       </c>
@@ -20080,9 +20334,12 @@
       <c r="H183" s="21" t="s">
         <v>1021</v>
       </c>
-      <c r="I183" s="35"/>
-    </row>
-    <row r="184" spans="1:9" ht="30">
+      <c r="I183" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J183" s="43"/>
+    </row>
+    <row r="184" spans="1:10" ht="30">
       <c r="A184" s="23" t="s">
         <v>946</v>
       </c>
@@ -20103,9 +20360,12 @@
       <c r="H184" s="13" t="s">
         <v>1021</v>
       </c>
-      <c r="I184" s="35"/>
-    </row>
-    <row r="185" spans="1:9">
+      <c r="I184" s="35" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J184" s="43"/>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185" s="18" t="s">
         <v>947</v>
       </c>
@@ -20126,9 +20386,11 @@
       <c r="H185" s="21" t="s">
         <v>624</v>
       </c>
-      <c r="I185" s="35"/>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="I185" s="35" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="75">
       <c r="A186" s="18" t="s">
         <v>947</v>
       </c>
@@ -20149,9 +20411,11 @@
       <c r="H186" s="21" t="s">
         <v>683</v>
       </c>
-      <c r="I186" s="35"/>
-    </row>
-    <row r="187" spans="1:9" ht="75">
+      <c r="I186" s="44" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" ht="75">
       <c r="A187" s="18" t="s">
         <v>947</v>
       </c>
@@ -20171,10 +20435,10 @@
         <v>951</v>
       </c>
       <c r="I187" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" ht="75">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" ht="75">
       <c r="A188" s="18" t="s">
         <v>947</v>
       </c>
@@ -20194,10 +20458,10 @@
         <v>951</v>
       </c>
       <c r="I188" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10">
       <c r="A189" s="18" t="s">
         <v>947</v>
       </c>
@@ -20219,10 +20483,10 @@
         <v>955</v>
       </c>
       <c r="I189" s="35" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10">
       <c r="A190" s="22" t="s">
         <v>958</v>
       </c>
@@ -20243,9 +20507,11 @@
       <c r="H190" s="21" t="s">
         <v>624</v>
       </c>
-      <c r="I190" s="35"/>
-    </row>
-    <row r="191" spans="1:9" ht="45">
+      <c r="I190" s="35" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="45">
       <c r="A191" s="22" t="s">
         <v>958</v>
       </c>
@@ -20267,10 +20533,10 @@
         <v>960</v>
       </c>
       <c r="I191" s="35" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10">
       <c r="A192" s="9" t="s">
         <v>958</v>
       </c>
@@ -20292,7 +20558,7 @@
         <v>963</v>
       </c>
       <c r="I192" s="35" t="s">
-        <v>1023</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="45">
@@ -20315,7 +20581,7 @@
         <v>966</v>
       </c>
       <c r="I193" s="35" t="s">
-        <v>1023</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="30">
@@ -20339,7 +20605,9 @@
       <c r="H194" s="21" t="s">
         <v>970</v>
       </c>
-      <c r="I194" s="35"/>
+      <c r="I194" s="35" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="195" spans="1:9" ht="30">
       <c r="A195" s="22" t="s">
@@ -20362,7 +20630,9 @@
       <c r="H195" s="21" t="s">
         <v>970</v>
       </c>
-      <c r="I195" s="35"/>
+      <c r="I195" s="35" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="196" spans="1:9">
       <c r="A196" s="22" t="s">
@@ -20385,9 +20655,11 @@
       <c r="H196" s="21" t="s">
         <v>973</v>
       </c>
-      <c r="I196" s="35"/>
-    </row>
-    <row r="197" spans="1:9" ht="30">
+      <c r="I196" s="35" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="90">
       <c r="A197" s="22" t="s">
         <v>974</v>
       </c>
@@ -20408,13 +20680,24 @@
       <c r="H197" s="21" t="s">
         <v>977</v>
       </c>
-      <c r="I197" s="35" t="s">
-        <v>1022</v>
+      <c r="I197" s="44" t="s">
+        <v>1067</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="12">
+    <mergeCell ref="J121:J123"/>
+    <mergeCell ref="J171:J184"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="J109:J112"/>
+    <mergeCell ref="J113:J115"/>
+    <mergeCell ref="J116:J117"/>
+    <mergeCell ref="J118:J120"/>
     <mergeCell ref="J87:J90"/>
+    <mergeCell ref="J79:J81"/>
+    <mergeCell ref="J93:J96"/>
+    <mergeCell ref="J97:J100"/>
+    <mergeCell ref="J101:J104"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>